<commit_message>
Fixed reader to return appropriate string for formula cell
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_format.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_format.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\workspace\exceltable\xlbean\src\test\java\com\xlbean\reader\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="3" r:id="rId1"/>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">result!$B$1:$D$68</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="113">
   <si>
     <t>format#date</t>
     <phoneticPr fontId="1"/>
@@ -357,42 +352,54 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Format to be standard and formula inside</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>formatStr#standardAndFormulaInside?type=string</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>format#standardAndFormulaInside</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>formatStr#number?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#currency?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#accounting?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#date?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#time?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#percentage?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#string?type=string</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>formatStr#user?type=string</t>
+  </si>
+  <si>
+    <t>####</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="46">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
@@ -488,7 +495,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -646,6 +653,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="216" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -954,7 +964,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -962,42 +972,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="1.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="20.25" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.08203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.58203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.875" customWidth="1"/>
     <col min="13" max="13" width="20.25" customWidth="1"/>
     <col min="14" max="14" width="34.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="15" max="15" width="6.875" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="34.08203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.83203125" customWidth="1"/>
+    <col min="17" max="17" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.83203125" customWidth="1"/>
+    <col min="20" max="20" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.875" customWidth="1"/>
     <col min="22" max="23" width="16" customWidth="1"/>
-    <col min="24" max="24" width="6.83203125" customWidth="1"/>
-    <col min="25" max="25" width="19.33203125" customWidth="1"/>
-    <col min="27" max="27" width="6.83203125" customWidth="1"/>
+    <col min="24" max="24" width="6.875" customWidth="1"/>
+    <col min="25" max="25" width="19.375" customWidth="1"/>
+    <col min="27" max="27" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
         <v>97</v>
@@ -1026,8 +1034,11 @@
       <c r="Y1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -1060,8 +1071,11 @@
         <v>41</v>
       </c>
       <c r="AA3" s="29"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1148,8 +1162,12 @@
         <f>VLOOKUP(Z4,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC4" t="str">
+        <f>"AAA"&amp;"BBB"</f>
+        <v>AAABBB</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C5">
         <v>2</v>
       </c>
@@ -1233,8 +1251,12 @@
         <f>VLOOKUP(Z5,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC5">
+        <f>1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C6">
         <v>3</v>
       </c>
@@ -1298,8 +1320,12 @@
         <f>VLOOKUP(Z6,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC6" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C7">
         <v>4</v>
       </c>
@@ -1353,8 +1379,15 @@
         <f>VLOOKUP(Z7,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC7">
+        <f>AE7</f>
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1408,8 +1441,15 @@
         <f>VLOOKUP(Z8,result!$D:$E,2,FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC8" t="str">
+        <f>AE8</f>
+        <v>1</v>
+      </c>
+      <c r="AE8" s="53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C9">
         <v>6</v>
       </c>
@@ -1454,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C10">
         <v>7</v>
       </c>
@@ -1499,7 +1539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C11">
         <v>8</v>
       </c>
@@ -1544,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C12">
         <v>9</v>
       </c>
@@ -1589,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C13">
         <v>10</v>
       </c>
@@ -1624,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C14">
         <v>11</v>
       </c>
@@ -1651,7 +1691,7 @@
       <c r="P14" s="40"/>
       <c r="Q14" s="40"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C15">
         <v>12</v>
       </c>
@@ -1678,7 +1718,7 @@
       <c r="P15" s="40"/>
       <c r="Q15" s="40"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
         <v>13</v>
       </c>
@@ -1695,7 +1735,7 @@
       <c r="P16" s="40"/>
       <c r="Q16" s="40"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C17">
         <v>14</v>
       </c>
@@ -1712,7 +1752,7 @@
       <c r="P17" s="40"/>
       <c r="Q17" s="40"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C18">
         <v>15</v>
       </c>
@@ -1729,69 +1769,67 @@
       <c r="P18" s="40"/>
       <c r="Q18" s="40"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="1.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="20.25" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.875" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="26.08203125" customWidth="1"/>
-    <col min="9" max="9" width="6.83203125" customWidth="1"/>
-    <col min="10" max="10" width="17.58203125" customWidth="1"/>
-    <col min="11" max="11" width="53.83203125" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" customWidth="1"/>
+    <col min="8" max="8" width="26.125" customWidth="1"/>
+    <col min="9" max="9" width="6.875" customWidth="1"/>
+    <col min="10" max="10" width="17.625" customWidth="1"/>
+    <col min="11" max="11" width="53.875" customWidth="1"/>
+    <col min="12" max="12" width="6.875" customWidth="1"/>
     <col min="13" max="13" width="20.25" customWidth="1"/>
     <col min="14" max="14" width="34.75" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" customWidth="1"/>
+    <col min="15" max="15" width="6.875" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="34.08203125" customWidth="1"/>
-    <col min="18" max="18" width="6.83203125" customWidth="1"/>
+    <col min="17" max="17" width="34.125" customWidth="1"/>
+    <col min="18" max="18" width="6.875" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="20" max="20" width="5.1640625" customWidth="1"/>
-    <col min="21" max="21" width="6.83203125" customWidth="1"/>
+    <col min="20" max="20" width="5.125" customWidth="1"/>
+    <col min="21" max="21" width="6.875" customWidth="1"/>
     <col min="22" max="23" width="16" customWidth="1"/>
-    <col min="24" max="24" width="6.83203125" customWidth="1"/>
-    <col min="25" max="25" width="19.33203125" customWidth="1"/>
-    <col min="27" max="27" width="6.83203125" customWidth="1"/>
+    <col min="24" max="24" width="6.875" customWidth="1"/>
+    <col min="25" max="25" width="19.375" customWidth="1"/>
+    <col min="27" max="27" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -1799,31 +1837,34 @@
         <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" t="s">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>109</v>
+      </c>
+      <c r="V1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC1" t="s">
         <v>101</v>
       </c>
-      <c r="J1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" t="s">
-        <v>103</v>
-      </c>
-      <c r="P1" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" t="s">
-        <v>105</v>
-      </c>
-      <c r="V1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -1856,8 +1897,11 @@
         <v>41</v>
       </c>
       <c r="AA3" s="29"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1944,8 +1988,12 @@
         <f>VLOOKUP(Z4,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC4" t="str">
+        <f>"AAA"&amp;"BBB"</f>
+        <v>AAABBB</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C5">
         <v>2</v>
       </c>
@@ -2029,8 +2077,12 @@
         <f>VLOOKUP(Z5,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC5">
+        <f>1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C6">
         <v>3</v>
       </c>
@@ -2094,8 +2146,12 @@
         <f>VLOOKUP(Z6,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC6" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C7">
         <v>4</v>
       </c>
@@ -2149,8 +2205,15 @@
         <f>VLOOKUP(Z7,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC7">
+        <f>AE7</f>
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C8">
         <v>5</v>
       </c>
@@ -2204,8 +2267,15 @@
         <f>VLOOKUP(Z8,result!$D:$E,2,FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC8" t="str">
+        <f>AE8</f>
+        <v>1</v>
+      </c>
+      <c r="AE8" s="53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C9">
         <v>6</v>
       </c>
@@ -2250,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C10">
         <v>7</v>
       </c>
@@ -2295,7 +2365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C11">
         <v>8</v>
       </c>
@@ -2340,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="C12">
         <v>9</v>
       </c>
@@ -2385,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C13">
         <v>10</v>
       </c>
@@ -2420,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C14">
         <v>11</v>
       </c>
@@ -2447,7 +2517,7 @@
       <c r="P14" s="40"/>
       <c r="Q14" s="40"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C15">
         <v>12</v>
       </c>
@@ -2474,7 +2544,7 @@
       <c r="P15" s="40"/>
       <c r="Q15" s="40"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
         <v>13</v>
       </c>
@@ -2491,7 +2561,7 @@
       <c r="P16" s="40"/>
       <c r="Q16" s="40"/>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C17">
         <v>14</v>
       </c>
@@ -2508,7 +2578,7 @@
       <c r="P17" s="40"/>
       <c r="Q17" s="40"/>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="C18">
         <v>15</v>
       </c>
@@ -2525,30 +2595,30 @@
       <c r="P18" s="40"/>
       <c r="Q18" s="40"/>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2556,16 +2626,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>64</v>
       </c>
@@ -2576,7 +2644,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="4" t="s">
         <v>71</v>
       </c>
@@ -2590,7 +2658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
         <v>71</v>
       </c>
@@ -2604,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4" t="s">
         <v>71</v>
       </c>
@@ -2618,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
@@ -2632,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="4" t="s">
         <v>71</v>
       </c>
@@ -2646,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
@@ -2660,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
         <v>71</v>
       </c>
@@ -2674,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4" t="s">
         <v>71</v>
       </c>
@@ -2688,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4" t="s">
         <v>77</v>
       </c>
@@ -2702,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4" t="s">
         <v>77</v>
       </c>
@@ -2716,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>77</v>
       </c>
@@ -2730,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4" t="s">
         <v>77</v>
       </c>
@@ -2744,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B14" s="4" t="s">
         <v>77</v>
       </c>
@@ -2758,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B15" s="4" t="s">
         <v>77</v>
       </c>
@@ -2772,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4" t="s">
         <v>77</v>
       </c>
@@ -2786,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="4" t="s">
         <v>77</v>
       </c>
@@ -2800,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B18" s="4" t="s">
         <v>72</v>
       </c>
@@ -2814,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4" t="s">
         <v>72</v>
       </c>
@@ -2828,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B20" s="4" t="s">
         <v>72</v>
       </c>
@@ -2842,7 +2910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="4" t="s">
         <v>72</v>
       </c>
@@ -2856,7 +2924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4" t="s">
         <v>72</v>
       </c>
@@ -2870,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="4" t="s">
         <v>72</v>
       </c>
@@ -2884,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B24" s="4" t="s">
         <v>78</v>
       </c>
@@ -2898,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="4" t="s">
         <v>78</v>
       </c>
@@ -2912,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B26" s="4" t="s">
         <v>78</v>
       </c>
@@ -2926,7 +2994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="4" t="s">
         <v>78</v>
       </c>
@@ -2940,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="4" t="s">
         <v>78</v>
       </c>
@@ -2954,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B29" s="4" t="s">
         <v>75</v>
       </c>
@@ -2968,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="4" t="s">
         <v>75</v>
       </c>
@@ -2982,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
@@ -2996,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" s="4" t="s">
         <v>75</v>
       </c>
@@ -3010,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B33" s="4" t="s">
         <v>75</v>
       </c>
@@ -3024,7 +3092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B34" s="4" t="s">
         <v>74</v>
       </c>
@@ -3038,7 +3106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B35" s="4" t="s">
         <v>74</v>
       </c>
@@ -3052,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B36" s="4" t="s">
         <v>74</v>
       </c>
@@ -3066,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B37" s="4" t="s">
         <v>74</v>
       </c>
@@ -3080,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B38" s="4" t="s">
         <v>79</v>
       </c>
@@ -3094,7 +3162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B39" s="4" t="s">
         <v>79</v>
       </c>
@@ -3108,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B40" s="4" t="s">
         <v>79</v>
       </c>
@@ -3122,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B41" s="4" t="s">
         <v>79</v>
       </c>
@@ -3136,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B42" s="4" t="s">
         <v>82</v>
       </c>
@@ -3150,7 +3218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B43" s="4" t="s">
         <v>82</v>
       </c>
@@ -3164,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B44" s="4" t="s">
         <v>82</v>
       </c>
@@ -3178,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B45" s="4" t="s">
         <v>82</v>
       </c>
@@ -3192,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B46" s="4" t="s">
         <v>83</v>
       </c>
@@ -3206,7 +3274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B47" s="4" t="s">
         <v>83</v>
       </c>
@@ -3220,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B48" s="4" t="s">
         <v>83</v>
       </c>
@@ -3234,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B49" s="4" t="s">
         <v>83</v>
       </c>
@@ -3248,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" s="4" t="s">
         <v>84</v>
       </c>
@@ -3262,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B51" s="4" t="s">
         <v>84</v>
       </c>
@@ -3276,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B52" s="4" t="s">
         <v>84</v>
       </c>
@@ -3290,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B53" s="4" t="s">
         <v>85</v>
       </c>
@@ -3304,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B54" s="4" t="s">
         <v>85</v>
       </c>
@@ -3318,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B55" s="4" t="s">
         <v>85</v>
       </c>
@@ -3332,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B56" s="4" t="s">
         <v>86</v>
       </c>
@@ -3346,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B57" s="4" t="s">
         <v>86</v>
       </c>
@@ -3360,7 +3428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B58" s="4" t="s">
         <v>87</v>
       </c>
@@ -3374,7 +3442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" s="4" t="s">
         <v>87</v>
       </c>
@@ -3388,7 +3456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B60" s="4" t="s">
         <v>88</v>
       </c>
@@ -3402,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B61" s="4" t="s">
         <v>88</v>
       </c>
@@ -3416,7 +3484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B62" s="4" t="s">
         <v>89</v>
       </c>
@@ -3430,7 +3498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B63" s="4" t="s">
         <v>89</v>
       </c>
@@ -3444,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B64" s="4" t="s">
         <v>90</v>
       </c>
@@ -3458,7 +3526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B65" s="4" t="s">
         <v>91</v>
       </c>
@@ -3472,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B66" s="4" t="s">
         <v>92</v>
       </c>
@@ -3486,7 +3554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B67" s="4" t="s">
         <v>93</v>
       </c>
@@ -3500,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" s="4" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Fixed date value format issue (value 0:00 become null)
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/reader/TestBook_format.xlsx
+++ b/src/test/resources/org/xlbean/reader/TestBook_format.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\reader\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="format" sheetId="3" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">result!$B$1:$D$68</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="113">
   <si>
     <t>format#date</t>
     <phoneticPr fontId="1"/>
@@ -399,7 +404,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="46">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="6" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
@@ -964,46 +969,46 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="1.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="20.25" customWidth="1"/>
-    <col min="6" max="6" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.875" customWidth="1"/>
+    <col min="8" max="8" width="26.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" customWidth="1"/>
     <col min="13" max="13" width="20.25" customWidth="1"/>
     <col min="14" max="14" width="34.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.875" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.875" customWidth="1"/>
+    <col min="17" max="17" width="34.08203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="20" max="20" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.875" customWidth="1"/>
+    <col min="20" max="20" width="5.08203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.83203125" customWidth="1"/>
     <col min="22" max="23" width="16" customWidth="1"/>
-    <col min="24" max="24" width="6.875" customWidth="1"/>
-    <col min="25" max="25" width="19.375" customWidth="1"/>
-    <col min="27" max="27" width="6.875" customWidth="1"/>
+    <col min="24" max="24" width="6.83203125" customWidth="1"/>
+    <col min="25" max="25" width="19.33203125" customWidth="1"/>
+    <col min="27" max="27" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -1038,7 +1043,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -1075,7 +1080,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1167,7 +1172,7 @@
         <v>AAABBB</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C5">
         <v>2</v>
       </c>
@@ -1256,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C6">
         <v>3</v>
       </c>
@@ -1310,6 +1315,12 @@
         <f>VLOOKUP(Q6,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
+      <c r="S6" s="47">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="Y6" s="50">
         <v>0.29097222222222224</v>
       </c>
@@ -1325,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C7">
         <v>4</v>
       </c>
@@ -1349,6 +1360,9 @@
         <f>VLOOKUP(H7,result!$D:$E,2,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="J7" s="38">
+        <v>0</v>
+      </c>
       <c r="M7" s="8">
         <v>42812</v>
       </c>
@@ -1387,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C8">
         <v>5</v>
       </c>
@@ -1449,7 +1463,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C9">
         <v>6</v>
       </c>
@@ -1494,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C10">
         <v>7</v>
       </c>
@@ -1539,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C11">
         <v>8</v>
       </c>
@@ -1584,7 +1598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C12">
         <v>9</v>
       </c>
@@ -1629,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C13">
         <v>10</v>
       </c>
@@ -1643,6 +1657,12 @@
         <f>VLOOKUP(E13,result!$D:$E,2,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G13" s="34">
+        <v>0</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>58</v>
+      </c>
       <c r="M13" s="14">
         <v>42812</v>
       </c>
@@ -1664,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C14">
         <v>11</v>
       </c>
@@ -1688,10 +1708,14 @@
         <f>VLOOKUP(N14,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-    </row>
-    <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="P14" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C15">
         <v>12</v>
       </c>
@@ -1718,10 +1742,16 @@
       <c r="P15" s="40"/>
       <c r="Q15" s="40"/>
     </row>
-    <row r="16" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
         <v>13</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
       <c r="M16" s="18">
         <v>42812</v>
       </c>
@@ -1735,7 +1765,7 @@
       <c r="P16" s="40"/>
       <c r="Q16" s="40"/>
     </row>
-    <row r="17" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C17">
         <v>14</v>
       </c>
@@ -1752,7 +1782,7 @@
       <c r="P17" s="40"/>
       <c r="Q17" s="40"/>
     </row>
-    <row r="18" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C18">
         <v>15</v>
       </c>
@@ -1769,23 +1799,33 @@
       <c r="P18" s="40"/>
       <c r="Q18" s="40"/>
     </row>
-    <row r="19" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-    </row>
-    <row r="20" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="M19" s="10">
+        <v>0</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20">
+        <v>17</v>
+      </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
     </row>
-    <row r="21" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
     </row>
-    <row r="22" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
     </row>
@@ -1797,39 +1837,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="1.25" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="5" width="20.25" customWidth="1"/>
-    <col min="6" max="6" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="26.125" customWidth="1"/>
-    <col min="9" max="9" width="6.875" customWidth="1"/>
-    <col min="10" max="10" width="17.625" customWidth="1"/>
-    <col min="11" max="11" width="53.875" customWidth="1"/>
-    <col min="12" max="12" width="6.875" customWidth="1"/>
+    <col min="8" max="8" width="26.08203125" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="17.58203125" customWidth="1"/>
+    <col min="11" max="11" width="53.83203125" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" customWidth="1"/>
     <col min="13" max="13" width="20.25" customWidth="1"/>
     <col min="14" max="14" width="34.75" customWidth="1"/>
-    <col min="15" max="15" width="6.875" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="34.125" customWidth="1"/>
-    <col min="18" max="18" width="6.875" customWidth="1"/>
+    <col min="17" max="17" width="34.08203125" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="20" max="20" width="5.125" customWidth="1"/>
-    <col min="21" max="21" width="6.875" customWidth="1"/>
+    <col min="20" max="20" width="5.08203125" customWidth="1"/>
+    <col min="21" max="21" width="6.83203125" customWidth="1"/>
     <col min="22" max="23" width="16" customWidth="1"/>
-    <col min="24" max="24" width="6.875" customWidth="1"/>
-    <col min="25" max="25" width="19.375" customWidth="1"/>
-    <col min="27" max="27" width="6.875" customWidth="1"/>
+    <col min="24" max="24" width="6.83203125" customWidth="1"/>
+    <col min="25" max="25" width="19.33203125" customWidth="1"/>
+    <col min="27" max="27" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>96</v>
       </c>
@@ -1864,7 +1906,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -1901,7 +1943,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1993,7 +2035,7 @@
         <v>AAABBB</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C5">
         <v>2</v>
       </c>
@@ -2082,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C6">
         <v>3</v>
       </c>
@@ -2136,6 +2178,12 @@
         <f>VLOOKUP(Q6,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
+      <c r="S6" s="47">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="Y6" s="50">
         <v>0.29097222222222224</v>
       </c>
@@ -2151,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C7">
         <v>4</v>
       </c>
@@ -2175,6 +2223,9 @@
         <f>VLOOKUP(H7,result!$D:$E,2,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="J7" s="38">
+        <v>0</v>
+      </c>
       <c r="M7" s="8">
         <v>42812</v>
       </c>
@@ -2213,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C8">
         <v>5</v>
       </c>
@@ -2275,7 +2326,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C9">
         <v>6</v>
       </c>
@@ -2320,7 +2371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C10">
         <v>7</v>
       </c>
@@ -2365,7 +2416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C11">
         <v>8</v>
       </c>
@@ -2410,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C12">
         <v>9</v>
       </c>
@@ -2455,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C13">
         <v>10</v>
       </c>
@@ -2469,6 +2520,12 @@
         <f>VLOOKUP(E13,result!$D:$E,2,FALSE)</f>
         <v>0</v>
       </c>
+      <c r="G13" s="34">
+        <v>0</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>58</v>
+      </c>
       <c r="M13" s="14">
         <v>42812</v>
       </c>
@@ -2490,7 +2547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C14">
         <v>11</v>
       </c>
@@ -2514,10 +2571,14 @@
         <f>VLOOKUP(N14,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-    </row>
-    <row r="15" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="P14" s="41">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C15">
         <v>12</v>
       </c>
@@ -2541,13 +2602,18 @@
         <f>VLOOKUP(N15,result!$D:$E,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="P15" s="40"/>
       <c r="Q15" s="40"/>
     </row>
-    <row r="16" spans="1:31" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
         <v>13</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
       <c r="M16" s="18">
         <v>42812</v>
       </c>
@@ -2561,7 +2627,7 @@
       <c r="P16" s="40"/>
       <c r="Q16" s="40"/>
     </row>
-    <row r="17" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C17">
         <v>14</v>
       </c>
@@ -2578,7 +2644,7 @@
       <c r="P17" s="40"/>
       <c r="Q17" s="40"/>
     </row>
-    <row r="18" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="C18">
         <v>15</v>
       </c>
@@ -2595,23 +2661,32 @@
       <c r="P18" s="40"/>
       <c r="Q18" s="40"/>
     </row>
-    <row r="19" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-    </row>
-    <row r="20" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="M20" s="17"/>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="M19" s="10">
+        <v>0</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20">
+        <v>17</v>
+      </c>
       <c r="N20" s="17"/>
     </row>
-    <row r="21" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
     </row>
-    <row r="22" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="3:17" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:17" x14ac:dyDescent="0.55000000000000004">
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
     </row>
@@ -2623,17 +2698,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>64</v>
       </c>
@@ -2644,7 +2719,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="4" t="s">
         <v>71</v>
       </c>
@@ -2658,7 +2733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="4" t="s">
         <v>71</v>
       </c>
@@ -2672,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4" t="s">
         <v>71</v>
       </c>
@@ -2686,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
@@ -2700,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4" t="s">
         <v>71</v>
       </c>
@@ -2714,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4" t="s">
         <v>71</v>
       </c>
@@ -2728,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
         <v>71</v>
       </c>
@@ -2742,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4" t="s">
         <v>71</v>
       </c>
@@ -2756,7 +2831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4" t="s">
         <v>77</v>
       </c>
@@ -2770,7 +2845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4" t="s">
         <v>77</v>
       </c>
@@ -2784,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>77</v>
       </c>
@@ -2798,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4" t="s">
         <v>77</v>
       </c>
@@ -2812,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4" t="s">
         <v>77</v>
       </c>
@@ -2826,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4" t="s">
         <v>77</v>
       </c>
@@ -2840,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4" t="s">
         <v>77</v>
       </c>
@@ -2854,7 +2929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="4" t="s">
         <v>77</v>
       </c>
@@ -2868,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="4" t="s">
         <v>72</v>
       </c>
@@ -2882,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4" t="s">
         <v>72</v>
       </c>
@@ -2896,7 +2971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4" t="s">
         <v>72</v>
       </c>
@@ -2910,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="4" t="s">
         <v>72</v>
       </c>
@@ -2924,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="4" t="s">
         <v>72</v>
       </c>
@@ -2938,7 +3013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="4" t="s">
         <v>72</v>
       </c>
@@ -2952,7 +3027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="4" t="s">
         <v>78</v>
       </c>
@@ -2966,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="4" t="s">
         <v>78</v>
       </c>
@@ -2980,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="4" t="s">
         <v>78</v>
       </c>
@@ -2994,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="4" t="s">
         <v>78</v>
       </c>
@@ -3008,7 +3083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="4" t="s">
         <v>78</v>
       </c>
@@ -3022,7 +3097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="4" t="s">
         <v>75</v>
       </c>
@@ -3036,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="4" t="s">
         <v>75</v>
       </c>
@@ -3050,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
@@ -3064,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="4" t="s">
         <v>75</v>
       </c>
@@ -3078,7 +3153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="4" t="s">
         <v>75</v>
       </c>
@@ -3092,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="4" t="s">
         <v>74</v>
       </c>
@@ -3106,7 +3181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="4" t="s">
         <v>74</v>
       </c>
@@ -3120,7 +3195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="4" t="s">
         <v>74</v>
       </c>
@@ -3134,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="4" t="s">
         <v>74</v>
       </c>
@@ -3148,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="4" t="s">
         <v>79</v>
       </c>
@@ -3162,7 +3237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="4" t="s">
         <v>79</v>
       </c>
@@ -3176,7 +3251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="4" t="s">
         <v>79</v>
       </c>
@@ -3190,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="4" t="s">
         <v>79</v>
       </c>
@@ -3204,7 +3279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="4" t="s">
         <v>82</v>
       </c>
@@ -3218,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="4" t="s">
         <v>82</v>
       </c>
@@ -3232,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="4" t="s">
         <v>82</v>
       </c>
@@ -3246,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="4" t="s">
         <v>82</v>
       </c>
@@ -3260,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="4" t="s">
         <v>83</v>
       </c>
@@ -3274,7 +3349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="4" t="s">
         <v>83</v>
       </c>
@@ -3288,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="4" t="s">
         <v>83</v>
       </c>
@@ -3302,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="4" t="s">
         <v>83</v>
       </c>
@@ -3316,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="4" t="s">
         <v>84</v>
       </c>
@@ -3330,7 +3405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="4" t="s">
         <v>84</v>
       </c>
@@ -3344,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="4" t="s">
         <v>84</v>
       </c>
@@ -3358,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="4" t="s">
         <v>85</v>
       </c>
@@ -3372,7 +3447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" s="4" t="s">
         <v>85</v>
       </c>
@@ -3386,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="4" t="s">
         <v>85</v>
       </c>
@@ -3400,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="4" t="s">
         <v>86</v>
       </c>
@@ -3414,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="4" t="s">
         <v>86</v>
       </c>
@@ -3428,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="4" t="s">
         <v>87</v>
       </c>
@@ -3442,7 +3517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="4" t="s">
         <v>87</v>
       </c>
@@ -3456,7 +3531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="4" t="s">
         <v>88</v>
       </c>
@@ -3470,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="4" t="s">
         <v>88</v>
       </c>
@@ -3484,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="4" t="s">
         <v>89</v>
       </c>
@@ -3498,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="4" t="s">
         <v>89</v>
       </c>
@@ -3512,7 +3587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="4" t="s">
         <v>90</v>
       </c>
@@ -3526,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" s="4" t="s">
         <v>91</v>
       </c>
@@ -3540,7 +3615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="4" t="s">
         <v>92</v>
       </c>
@@ -3554,7 +3629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="4" t="s">
         <v>93</v>
       </c>
@@ -3568,7 +3643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="4" t="s">
         <v>94</v>
       </c>
@@ -3583,7 +3658,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D68"/>
+  <autoFilter ref="B1:D68" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>